<commit_message>
docs: add VideoA Bright Adjust
</commit_message>
<xml_diff>
--- a/docs/v8/memory-map.xlsx
+++ b/docs/v8/memory-map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpotvin/Git/edirol-midi-dump/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpotvin/Git/edirol-midi-dump/docs/v8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EE8708-BC8E-754C-9A40-60FD91C45C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C323E77-B9BF-D241-AFF4-6DC732429A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{23572B00-E77A-A64D-AC8F-FBD0BFC92319}"/>
+    <workbookView xWindow="8480" yWindow="-25060" windowWidth="28040" windowHeight="17440" xr2:uid="{23572B00-E77A-A64D-AC8F-FBD0BFC92319}"/>
   </bookViews>
   <sheets>
     <sheet name="V-8 Memory Map" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="661">
   <si>
     <t>200100</t>
   </si>
@@ -1437,592 +1437,604 @@
     <t>00 is negative, 01 is positive. See address 206007.</t>
   </si>
   <si>
-    <t>20010a</t>
-  </si>
-  <si>
-    <t>20010b</t>
-  </si>
-  <si>
-    <t>20010c</t>
-  </si>
-  <si>
-    <t>20010d</t>
-  </si>
-  <si>
-    <t>20010e</t>
-  </si>
-  <si>
-    <t>20010f</t>
-  </si>
-  <si>
-    <t>20011a</t>
-  </si>
-  <si>
-    <t>20020a</t>
-  </si>
-  <si>
-    <t>20020b</t>
-  </si>
-  <si>
-    <t>20020c</t>
-  </si>
-  <si>
-    <t>20020d</t>
-  </si>
-  <si>
-    <t>20020e</t>
-  </si>
-  <si>
-    <t>20020f</t>
-  </si>
-  <si>
-    <t>20021a</t>
-  </si>
-  <si>
-    <t>20030a</t>
-  </si>
-  <si>
-    <t>20030b</t>
-  </si>
-  <si>
-    <t>20030c</t>
-  </si>
-  <si>
-    <t>20030d</t>
-  </si>
-  <si>
-    <t>20030e</t>
-  </si>
-  <si>
-    <t>20030f</t>
-  </si>
-  <si>
-    <t>20031a</t>
-  </si>
-  <si>
-    <t>20040a</t>
-  </si>
-  <si>
-    <t>20040b</t>
-  </si>
-  <si>
-    <t>20040c</t>
-  </si>
-  <si>
-    <t>20040d</t>
-  </si>
-  <si>
-    <t>20040e</t>
-  </si>
-  <si>
-    <t>20040f</t>
-  </si>
-  <si>
-    <t>20041a</t>
-  </si>
-  <si>
-    <t>20050a</t>
-  </si>
-  <si>
-    <t>20050b</t>
-  </si>
-  <si>
-    <t>20050c</t>
-  </si>
-  <si>
-    <t>20050d</t>
-  </si>
-  <si>
-    <t>20050e</t>
-  </si>
-  <si>
-    <t>20050f</t>
-  </si>
-  <si>
-    <t>20051a</t>
-  </si>
-  <si>
-    <t>20060a</t>
-  </si>
-  <si>
-    <t>20060b</t>
-  </si>
-  <si>
-    <t>20060c</t>
-  </si>
-  <si>
-    <t>20060d</t>
-  </si>
-  <si>
-    <t>20060e</t>
-  </si>
-  <si>
-    <t>20060f</t>
-  </si>
-  <si>
-    <t>20061a</t>
-  </si>
-  <si>
-    <t>20070a</t>
-  </si>
-  <si>
-    <t>20070b</t>
-  </si>
-  <si>
-    <t>20070c</t>
-  </si>
-  <si>
-    <t>20070d</t>
-  </si>
-  <si>
-    <t>20070e</t>
-  </si>
-  <si>
-    <t>20070f</t>
-  </si>
-  <si>
-    <t>20071a</t>
-  </si>
-  <si>
-    <t>20100a</t>
-  </si>
-  <si>
-    <t>20100b</t>
-  </si>
-  <si>
-    <t>20100c</t>
-  </si>
-  <si>
-    <t>20100d</t>
-  </si>
-  <si>
-    <t>20100e</t>
-  </si>
-  <si>
-    <t>20100f</t>
-  </si>
-  <si>
-    <t>20110a</t>
-  </si>
-  <si>
-    <t>20110b</t>
-  </si>
-  <si>
-    <t>20110c</t>
-  </si>
-  <si>
-    <t>20110d</t>
-  </si>
-  <si>
-    <t>20110e</t>
-  </si>
-  <si>
-    <t>20110f</t>
-  </si>
-  <si>
-    <t>20200a</t>
-  </si>
-  <si>
-    <t>20200b</t>
-  </si>
-  <si>
-    <t>20200c</t>
-  </si>
-  <si>
-    <t>20200d</t>
-  </si>
-  <si>
-    <t>20200e</t>
-  </si>
-  <si>
-    <t>20200f</t>
-  </si>
-  <si>
-    <t>20210a</t>
-  </si>
-  <si>
-    <t>20210b</t>
-  </si>
-  <si>
-    <t>20210c</t>
-  </si>
-  <si>
-    <t>20210d</t>
-  </si>
-  <si>
-    <t>20210e</t>
-  </si>
-  <si>
-    <t>20210f</t>
-  </si>
-  <si>
-    <t>20220a</t>
-  </si>
-  <si>
-    <t>20220b</t>
-  </si>
-  <si>
-    <t>20220c</t>
-  </si>
-  <si>
-    <t>20220d</t>
-  </si>
-  <si>
-    <t>20220e</t>
-  </si>
-  <si>
-    <t>20220f</t>
-  </si>
-  <si>
-    <t>20230a</t>
-  </si>
-  <si>
-    <t>20230b</t>
-  </si>
-  <si>
-    <t>20230c</t>
-  </si>
-  <si>
-    <t>20230d</t>
-  </si>
-  <si>
-    <t>20230e</t>
-  </si>
-  <si>
-    <t>20230f</t>
-  </si>
-  <si>
-    <t>20300a</t>
-  </si>
-  <si>
-    <t>20300b</t>
-  </si>
-  <si>
-    <t>20300c</t>
-  </si>
-  <si>
-    <t>20300d</t>
-  </si>
-  <si>
-    <t>20300e</t>
-  </si>
-  <si>
-    <t>20300f</t>
-  </si>
-  <si>
-    <t>20310a</t>
-  </si>
-  <si>
-    <t>20310b</t>
-  </si>
-  <si>
-    <t>20310c</t>
-  </si>
-  <si>
-    <t>20310d</t>
-  </si>
-  <si>
-    <t>20310e</t>
-  </si>
-  <si>
-    <t>20310f</t>
-  </si>
-  <si>
-    <t>20320a</t>
-  </si>
-  <si>
-    <t>20320b</t>
-  </si>
-  <si>
-    <t>20320c</t>
-  </si>
-  <si>
-    <t>20320d</t>
-  </si>
-  <si>
-    <t>20320e</t>
-  </si>
-  <si>
-    <t>20320f</t>
-  </si>
-  <si>
-    <t>20330a</t>
-  </si>
-  <si>
-    <t>20330b</t>
-  </si>
-  <si>
-    <t>20330c</t>
-  </si>
-  <si>
-    <t>20330d</t>
-  </si>
-  <si>
-    <t>20330e</t>
-  </si>
-  <si>
-    <t>20330f</t>
-  </si>
-  <si>
-    <t>20340a</t>
-  </si>
-  <si>
-    <t>20340b</t>
-  </si>
-  <si>
-    <t>20340c</t>
-  </si>
-  <si>
-    <t>20340d</t>
-  </si>
-  <si>
-    <t>20340e</t>
-  </si>
-  <si>
-    <t>20340f</t>
-  </si>
-  <si>
-    <t>20350a</t>
-  </si>
-  <si>
-    <t>20350b</t>
-  </si>
-  <si>
-    <t>20350c</t>
-  </si>
-  <si>
-    <t>20350d</t>
-  </si>
-  <si>
-    <t>20350e</t>
-  </si>
-  <si>
-    <t>20350f</t>
-  </si>
-  <si>
-    <t>20360a</t>
-  </si>
-  <si>
-    <t>20360b</t>
-  </si>
-  <si>
-    <t>20360c</t>
-  </si>
-  <si>
-    <t>20360d</t>
-  </si>
-  <si>
-    <t>20360e</t>
-  </si>
-  <si>
-    <t>20360f</t>
-  </si>
-  <si>
-    <t>20370a</t>
-  </si>
-  <si>
-    <t>20370b</t>
-  </si>
-  <si>
-    <t>20370c</t>
-  </si>
-  <si>
-    <t>20370d</t>
-  </si>
-  <si>
-    <t>20370e</t>
-  </si>
-  <si>
-    <t>20370f</t>
-  </si>
-  <si>
-    <t>20400a</t>
-  </si>
-  <si>
-    <t>20400b</t>
-  </si>
-  <si>
-    <t>20400c</t>
-  </si>
-  <si>
-    <t>20400d</t>
-  </si>
-  <si>
-    <t>20400e</t>
-  </si>
-  <si>
-    <t>20400f</t>
-  </si>
-  <si>
-    <t>20500a</t>
-  </si>
-  <si>
-    <t>20500b</t>
-  </si>
-  <si>
-    <t>20500c</t>
-  </si>
-  <si>
-    <t>20500d</t>
-  </si>
-  <si>
-    <t>20500e</t>
-  </si>
-  <si>
-    <t>20500f</t>
-  </si>
-  <si>
-    <t>20501a</t>
-  </si>
-  <si>
-    <t>20501b</t>
-  </si>
-  <si>
-    <t>20501c</t>
-  </si>
-  <si>
-    <t>20501d</t>
-  </si>
-  <si>
-    <t>20501e</t>
-  </si>
-  <si>
-    <t>20501f</t>
-  </si>
-  <si>
-    <t>20600a</t>
-  </si>
-  <si>
-    <t>20600b</t>
-  </si>
-  <si>
-    <t>20600c</t>
-  </si>
-  <si>
-    <t>20600d</t>
-  </si>
-  <si>
-    <t>20600e</t>
-  </si>
-  <si>
-    <t>20600f</t>
-  </si>
-  <si>
-    <t>20601a</t>
-  </si>
-  <si>
-    <t>20601b</t>
-  </si>
-  <si>
-    <t>20601c</t>
-  </si>
-  <si>
-    <t>20601d</t>
-  </si>
-  <si>
-    <t>20601e</t>
-  </si>
-  <si>
-    <t>20601f</t>
-  </si>
-  <si>
-    <t>20602a</t>
-  </si>
-  <si>
-    <t>20602b</t>
-  </si>
-  <si>
-    <t>20602c</t>
-  </si>
-  <si>
-    <t>20602d</t>
-  </si>
-  <si>
-    <t>20602e</t>
-  </si>
-  <si>
-    <t>20602f</t>
-  </si>
-  <si>
-    <t>2f7f00</t>
-  </si>
-  <si>
-    <t>3d</t>
-  </si>
-  <si>
-    <t>0c</t>
-  </si>
-  <si>
-    <t>5d</t>
-  </si>
-  <si>
-    <t>5f</t>
-  </si>
-  <si>
-    <t>3b</t>
-  </si>
-  <si>
-    <t>1b</t>
-  </si>
-  <si>
-    <t>7d</t>
-  </si>
-  <si>
-    <t>5c</t>
-  </si>
-  <si>
-    <t>2b</t>
-  </si>
-  <si>
-    <t>4d</t>
-  </si>
-  <si>
-    <t>5b</t>
-  </si>
-  <si>
-    <t>0b</t>
-  </si>
-  <si>
-    <t>0d</t>
-  </si>
-  <si>
-    <t>0f</t>
-  </si>
-  <si>
-    <t>6a</t>
-  </si>
-  <si>
-    <t>7e</t>
-  </si>
-  <si>
-    <t>1f</t>
-  </si>
-  <si>
-    <t>2e</t>
-  </si>
-  <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>5e</t>
-  </si>
-  <si>
-    <t>4e</t>
-  </si>
-  <si>
-    <t>1a</t>
-  </si>
-  <si>
-    <t>4f</t>
-  </si>
-  <si>
-    <t>0e</t>
-  </si>
-  <si>
-    <t>0a</t>
-  </si>
-  <si>
-    <t>7-bit signed integer, 0 value is 00 with byte 206006 set to 01. Negative values start at 7f.</t>
+    <t>VideoA Bright Adjust</t>
+  </si>
+  <si>
+    <t>VideoA Beight Adjust</t>
+  </si>
+  <si>
+    <t>00 is negative, 01 is positive. See address 206005.</t>
+  </si>
+  <si>
+    <t>7-bit signed integer, 0 value is 00 with byte 206004 set to 01. 3Dh=61d 44h=68d (127-59?)</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>5F</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>7D</t>
+  </si>
+  <si>
+    <t>5C</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>5E</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>0E</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>20010A</t>
+  </si>
+  <si>
+    <t>20010B</t>
+  </si>
+  <si>
+    <t>20010C</t>
+  </si>
+  <si>
+    <t>20010D</t>
+  </si>
+  <si>
+    <t>20010E</t>
+  </si>
+  <si>
+    <t>20010F</t>
+  </si>
+  <si>
+    <t>20011A</t>
+  </si>
+  <si>
+    <t>20020A</t>
+  </si>
+  <si>
+    <t>20020B</t>
+  </si>
+  <si>
+    <t>20020C</t>
+  </si>
+  <si>
+    <t>20020D</t>
+  </si>
+  <si>
+    <t>20020E</t>
+  </si>
+  <si>
+    <t>20020F</t>
+  </si>
+  <si>
+    <t>20021A</t>
+  </si>
+  <si>
+    <t>20030A</t>
+  </si>
+  <si>
+    <t>20030B</t>
+  </si>
+  <si>
+    <t>20030C</t>
+  </si>
+  <si>
+    <t>20030D</t>
+  </si>
+  <si>
+    <t>20030E</t>
+  </si>
+  <si>
+    <t>20030F</t>
+  </si>
+  <si>
+    <t>20031A</t>
+  </si>
+  <si>
+    <t>20040A</t>
+  </si>
+  <si>
+    <t>20040B</t>
+  </si>
+  <si>
+    <t>20040C</t>
+  </si>
+  <si>
+    <t>20040D</t>
+  </si>
+  <si>
+    <t>20040E</t>
+  </si>
+  <si>
+    <t>20040F</t>
+  </si>
+  <si>
+    <t>20041A</t>
+  </si>
+  <si>
+    <t>20050A</t>
+  </si>
+  <si>
+    <t>20050B</t>
+  </si>
+  <si>
+    <t>20050C</t>
+  </si>
+  <si>
+    <t>20050D</t>
+  </si>
+  <si>
+    <t>20050E</t>
+  </si>
+  <si>
+    <t>20050F</t>
+  </si>
+  <si>
+    <t>20051A</t>
+  </si>
+  <si>
+    <t>20060A</t>
+  </si>
+  <si>
+    <t>20060B</t>
+  </si>
+  <si>
+    <t>20060C</t>
+  </si>
+  <si>
+    <t>20060D</t>
+  </si>
+  <si>
+    <t>20060E</t>
+  </si>
+  <si>
+    <t>20060F</t>
+  </si>
+  <si>
+    <t>20061A</t>
+  </si>
+  <si>
+    <t>20070A</t>
+  </si>
+  <si>
+    <t>20070B</t>
+  </si>
+  <si>
+    <t>20070C</t>
+  </si>
+  <si>
+    <t>20070D</t>
+  </si>
+  <si>
+    <t>20070E</t>
+  </si>
+  <si>
+    <t>20070F</t>
+  </si>
+  <si>
+    <t>20071A</t>
+  </si>
+  <si>
+    <t>20100A</t>
+  </si>
+  <si>
+    <t>20100B</t>
+  </si>
+  <si>
+    <t>20100C</t>
+  </si>
+  <si>
+    <t>20100D</t>
+  </si>
+  <si>
+    <t>20100E</t>
+  </si>
+  <si>
+    <t>20100F</t>
+  </si>
+  <si>
+    <t>20110A</t>
+  </si>
+  <si>
+    <t>20110B</t>
+  </si>
+  <si>
+    <t>20110C</t>
+  </si>
+  <si>
+    <t>20110D</t>
+  </si>
+  <si>
+    <t>20110E</t>
+  </si>
+  <si>
+    <t>20110F</t>
+  </si>
+  <si>
+    <t>20200A</t>
+  </si>
+  <si>
+    <t>20200B</t>
+  </si>
+  <si>
+    <t>20200C</t>
+  </si>
+  <si>
+    <t>20200D</t>
+  </si>
+  <si>
+    <t>20200E</t>
+  </si>
+  <si>
+    <t>20200F</t>
+  </si>
+  <si>
+    <t>20210A</t>
+  </si>
+  <si>
+    <t>20210B</t>
+  </si>
+  <si>
+    <t>20210C</t>
+  </si>
+  <si>
+    <t>20210D</t>
+  </si>
+  <si>
+    <t>20210E</t>
+  </si>
+  <si>
+    <t>20210F</t>
+  </si>
+  <si>
+    <t>20220A</t>
+  </si>
+  <si>
+    <t>20220B</t>
+  </si>
+  <si>
+    <t>20220C</t>
+  </si>
+  <si>
+    <t>20220D</t>
+  </si>
+  <si>
+    <t>20220E</t>
+  </si>
+  <si>
+    <t>20220F</t>
+  </si>
+  <si>
+    <t>20230A</t>
+  </si>
+  <si>
+    <t>20230B</t>
+  </si>
+  <si>
+    <t>20230C</t>
+  </si>
+  <si>
+    <t>20230D</t>
+  </si>
+  <si>
+    <t>20230E</t>
+  </si>
+  <si>
+    <t>20230F</t>
+  </si>
+  <si>
+    <t>20300A</t>
+  </si>
+  <si>
+    <t>20300B</t>
+  </si>
+  <si>
+    <t>20300C</t>
+  </si>
+  <si>
+    <t>20300D</t>
+  </si>
+  <si>
+    <t>20300E</t>
+  </si>
+  <si>
+    <t>20300F</t>
+  </si>
+  <si>
+    <t>20310A</t>
+  </si>
+  <si>
+    <t>20310B</t>
+  </si>
+  <si>
+    <t>20310C</t>
+  </si>
+  <si>
+    <t>20310D</t>
+  </si>
+  <si>
+    <t>20310E</t>
+  </si>
+  <si>
+    <t>20310F</t>
+  </si>
+  <si>
+    <t>20320A</t>
+  </si>
+  <si>
+    <t>20320B</t>
+  </si>
+  <si>
+    <t>20320C</t>
+  </si>
+  <si>
+    <t>20320D</t>
+  </si>
+  <si>
+    <t>20320E</t>
+  </si>
+  <si>
+    <t>20320F</t>
+  </si>
+  <si>
+    <t>20330A</t>
+  </si>
+  <si>
+    <t>20330B</t>
+  </si>
+  <si>
+    <t>20330C</t>
+  </si>
+  <si>
+    <t>20330D</t>
+  </si>
+  <si>
+    <t>20330E</t>
+  </si>
+  <si>
+    <t>20330F</t>
+  </si>
+  <si>
+    <t>20340A</t>
+  </si>
+  <si>
+    <t>20340B</t>
+  </si>
+  <si>
+    <t>20340C</t>
+  </si>
+  <si>
+    <t>20340D</t>
+  </si>
+  <si>
+    <t>20340E</t>
+  </si>
+  <si>
+    <t>20340F</t>
+  </si>
+  <si>
+    <t>20350A</t>
+  </si>
+  <si>
+    <t>20350B</t>
+  </si>
+  <si>
+    <t>20350C</t>
+  </si>
+  <si>
+    <t>20350D</t>
+  </si>
+  <si>
+    <t>20350E</t>
+  </si>
+  <si>
+    <t>20350F</t>
+  </si>
+  <si>
+    <t>20360A</t>
+  </si>
+  <si>
+    <t>20360B</t>
+  </si>
+  <si>
+    <t>20360C</t>
+  </si>
+  <si>
+    <t>20360D</t>
+  </si>
+  <si>
+    <t>20360E</t>
+  </si>
+  <si>
+    <t>20360F</t>
+  </si>
+  <si>
+    <t>20370A</t>
+  </si>
+  <si>
+    <t>20370B</t>
+  </si>
+  <si>
+    <t>20370C</t>
+  </si>
+  <si>
+    <t>20370D</t>
+  </si>
+  <si>
+    <t>20370E</t>
+  </si>
+  <si>
+    <t>20370F</t>
+  </si>
+  <si>
+    <t>20400A</t>
+  </si>
+  <si>
+    <t>20400B</t>
+  </si>
+  <si>
+    <t>20400C</t>
+  </si>
+  <si>
+    <t>20400D</t>
+  </si>
+  <si>
+    <t>20400E</t>
+  </si>
+  <si>
+    <t>20400F</t>
+  </si>
+  <si>
+    <t>20500A</t>
+  </si>
+  <si>
+    <t>20500B</t>
+  </si>
+  <si>
+    <t>20500C</t>
+  </si>
+  <si>
+    <t>20500D</t>
+  </si>
+  <si>
+    <t>20500E</t>
+  </si>
+  <si>
+    <t>20500F</t>
+  </si>
+  <si>
+    <t>20501A</t>
+  </si>
+  <si>
+    <t>20501B</t>
+  </si>
+  <si>
+    <t>20501C</t>
+  </si>
+  <si>
+    <t>20501D</t>
+  </si>
+  <si>
+    <t>20501E</t>
+  </si>
+  <si>
+    <t>20501F</t>
+  </si>
+  <si>
+    <t>20600A</t>
+  </si>
+  <si>
+    <t>20600B</t>
+  </si>
+  <si>
+    <t>20600C</t>
+  </si>
+  <si>
+    <t>20600D</t>
+  </si>
+  <si>
+    <t>20600E</t>
+  </si>
+  <si>
+    <t>20600F</t>
+  </si>
+  <si>
+    <t>20601A</t>
+  </si>
+  <si>
+    <t>20601B</t>
+  </si>
+  <si>
+    <t>20601C</t>
+  </si>
+  <si>
+    <t>20601D</t>
+  </si>
+  <si>
+    <t>20601E</t>
+  </si>
+  <si>
+    <t>20601F</t>
+  </si>
+  <si>
+    <t>20602A</t>
+  </si>
+  <si>
+    <t>20602B</t>
+  </si>
+  <si>
+    <t>20602C</t>
+  </si>
+  <si>
+    <t>20602D</t>
+  </si>
+  <si>
+    <t>20602E</t>
+  </si>
+  <si>
+    <t>20602F</t>
+  </si>
+  <si>
+    <t>2F7F00</t>
+  </si>
+  <si>
+    <t>7-bit signed integer, 0 value is 00 with byte 206006 set to 01. Negative values start at 7F.</t>
   </si>
 </sst>
 </file>
@@ -2381,8 +2393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46592BD5-1FB7-0E44-9287-ABB0C556451D}">
   <dimension ref="A1:F577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
-      <selection activeCell="D534" sqref="D534"/>
+    <sheetView tabSelected="1" topLeftCell="A517" workbookViewId="0">
+      <selection activeCell="E537" sqref="E537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2443,7 +2455,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>631</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2496,7 +2508,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>461</v>
+        <v>490</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
@@ -2504,7 +2516,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>462</v>
+        <v>491</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -2512,7 +2524,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>463</v>
+        <v>492</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -2520,15 +2532,15 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>464</v>
+        <v>493</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>632</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>465</v>
+        <v>494</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
@@ -2536,7 +2548,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>466</v>
+        <v>495</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
@@ -2555,7 +2567,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>633</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
@@ -2571,7 +2583,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
@@ -2587,7 +2599,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>632</v>
+        <v>466</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
@@ -2624,7 +2636,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>467</v>
+        <v>496</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>27</v>
@@ -2691,7 +2703,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>635</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
@@ -2712,7 +2724,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>468</v>
+        <v>497</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
@@ -2720,15 +2732,15 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>469</v>
+        <v>498</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>636</v>
+        <v>470</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>470</v>
+        <v>499</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>1</v>
@@ -2736,15 +2748,15 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
+        <v>500</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>472</v>
+        <v>501</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>1</v>
@@ -2752,7 +2764,7 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>473</v>
+        <v>502</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>41</v>
@@ -2787,7 +2799,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
@@ -2840,7 +2852,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>474</v>
+        <v>503</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>27</v>
@@ -2875,7 +2887,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>638</v>
+        <v>472</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.2">
@@ -2928,7 +2940,7 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>475</v>
+        <v>504</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>1</v>
@@ -2936,15 +2948,15 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>476</v>
+        <v>505</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>636</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>477</v>
+        <v>506</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>1</v>
@@ -2952,15 +2964,15 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>478</v>
+        <v>507</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>637</v>
+        <v>471</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>479</v>
+        <v>508</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>1</v>
@@ -2968,7 +2980,7 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>480</v>
+        <v>509</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>41</v>
@@ -3003,7 +3015,7 @@
         <v>68</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.2">
@@ -3056,7 +3068,7 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>481</v>
+        <v>510</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>27</v>
@@ -3091,7 +3103,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>639</v>
+        <v>473</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.2">
@@ -3139,12 +3151,12 @@
         <v>87</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>640</v>
+        <v>474</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>482</v>
+        <v>511</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>1</v>
@@ -3152,15 +3164,15 @@
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>483</v>
+        <v>512</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>641</v>
+        <v>475</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>484</v>
+        <v>513</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>15</v>
@@ -3168,15 +3180,15 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>485</v>
+        <v>514</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>632</v>
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>1</v>
@@ -3184,10 +3196,10 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>487</v>
+        <v>516</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.2">
@@ -3219,7 +3231,7 @@
         <v>91</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.2">
@@ -3272,7 +3284,7 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>488</v>
+        <v>517</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>27</v>
@@ -3323,7 +3335,7 @@
         <v>104</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>638</v>
+        <v>472</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.2">
@@ -3339,7 +3351,7 @@
         <v>106</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.2">
@@ -3360,7 +3372,7 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>489</v>
+        <v>518</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1</v>
@@ -3368,7 +3380,7 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>490</v>
+        <v>519</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>14</v>
@@ -3376,7 +3388,7 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>491</v>
+        <v>520</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>1</v>
@@ -3384,7 +3396,7 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>492</v>
+        <v>521</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>13</v>
@@ -3392,7 +3404,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>493</v>
+        <v>522</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>15</v>
@@ -3400,10 +3412,10 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>494</v>
+        <v>523</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>643</v>
+        <v>477</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.2">
@@ -3488,7 +3500,7 @@
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>495</v>
+        <v>524</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>27</v>
@@ -3576,7 +3588,7 @@
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>496</v>
+        <v>525</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>1</v>
@@ -3584,7 +3596,7 @@
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>497</v>
+        <v>526</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>14</v>
@@ -3592,7 +3604,7 @@
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>498</v>
+        <v>527</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>1</v>
@@ -3600,7 +3612,7 @@
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>499</v>
+        <v>528</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>40</v>
@@ -3608,7 +3620,7 @@
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>500</v>
+        <v>529</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>1</v>
@@ -3616,7 +3628,7 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>501</v>
+        <v>530</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>1</v>
@@ -3635,7 +3647,7 @@
         <v>134</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>633</v>
+        <v>467</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.2">
@@ -3651,7 +3663,7 @@
         <v>136</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.2">
@@ -3667,7 +3679,7 @@
         <v>138</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>644</v>
+        <v>478</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.2">
@@ -3704,7 +3716,7 @@
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>502</v>
+        <v>531</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>27</v>
@@ -3755,7 +3767,7 @@
         <v>148</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>645</v>
+        <v>479</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.2">
@@ -3771,7 +3783,7 @@
         <v>150</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.2">
@@ -3792,7 +3804,7 @@
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>503</v>
+        <v>532</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>1</v>
@@ -3800,7 +3812,7 @@
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>504</v>
+        <v>533</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>14</v>
@@ -3808,7 +3820,7 @@
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>505</v>
+        <v>534</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>1</v>
@@ -3816,15 +3828,15 @@
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>506</v>
+        <v>535</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>637</v>
+        <v>471</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>507</v>
+        <v>536</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>15</v>
@@ -3832,10 +3844,10 @@
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>508</v>
+        <v>537</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>632</v>
+        <v>466</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.2">
@@ -3867,7 +3879,7 @@
         <v>156</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.2">
@@ -3883,7 +3895,7 @@
         <v>158</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>643</v>
+        <v>477</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.2">
@@ -3920,7 +3932,7 @@
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>509</v>
+        <v>538</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>59</v>
@@ -3939,7 +3951,7 @@
         <v>164</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>646</v>
+        <v>480</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.2">
@@ -3971,7 +3983,7 @@
         <v>169</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>645</v>
+        <v>479</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.2">
@@ -4008,7 +4020,7 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>510</v>
+        <v>539</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>1</v>
@@ -4016,7 +4028,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>511</v>
+        <v>540</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>1</v>
@@ -4024,7 +4036,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>512</v>
+        <v>541</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>1</v>
@@ -4032,15 +4044,15 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>513</v>
+        <v>542</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>647</v>
+        <v>481</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>514</v>
+        <v>543</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>1</v>
@@ -4048,7 +4060,7 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>515</v>
+        <v>544</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>1</v>
@@ -4147,7 +4159,7 @@
         <v>185</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>636</v>
+        <v>470</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.2">
@@ -4195,7 +4207,7 @@
         <v>192</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>648</v>
+        <v>482</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.2">
@@ -4216,7 +4228,7 @@
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>516</v>
+        <v>545</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>1</v>
@@ -4224,7 +4236,7 @@
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>517</v>
+        <v>546</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>1</v>
@@ -4232,7 +4244,7 @@
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>518</v>
+        <v>547</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>1</v>
@@ -4240,15 +4252,15 @@
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>519</v>
+        <v>548</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>647</v>
+        <v>481</v>
       </c>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>520</v>
+        <v>549</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>1</v>
@@ -4256,7 +4268,7 @@
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>1</v>
@@ -4371,7 +4383,7 @@
         <v>209</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>633</v>
+        <v>467</v>
       </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.2">
@@ -4387,7 +4399,7 @@
         <v>211</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>641</v>
+        <v>475</v>
       </c>
     </row>
     <row r="249" spans="2:3" x14ac:dyDescent="0.2">
@@ -4403,7 +4415,7 @@
         <v>213</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>649</v>
+        <v>483</v>
       </c>
     </row>
     <row r="251" spans="2:3" x14ac:dyDescent="0.2">
@@ -4419,12 +4431,12 @@
         <v>215</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>638</v>
+        <v>472</v>
       </c>
     </row>
     <row r="253" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>522</v>
+        <v>551</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>1</v>
@@ -4432,15 +4444,15 @@
     </row>
     <row r="254" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>523</v>
+        <v>552</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>650</v>
+        <v>484</v>
       </c>
     </row>
     <row r="255" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>524</v>
+        <v>553</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>1</v>
@@ -4448,15 +4460,15 @@
     </row>
     <row r="256" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>525</v>
+        <v>554</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>634</v>
+        <v>468</v>
       </c>
     </row>
     <row r="257" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>526</v>
+        <v>555</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>1</v>
@@ -4464,7 +4476,7 @@
     </row>
     <row r="258" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>527</v>
+        <v>556</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>207</v>
@@ -4523,7 +4535,7 @@
         <v>222</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="266" spans="2:3" x14ac:dyDescent="0.2">
@@ -4539,7 +4551,7 @@
         <v>224</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>632</v>
+        <v>466</v>
       </c>
     </row>
     <row r="268" spans="2:3" x14ac:dyDescent="0.2">
@@ -4560,7 +4572,7 @@
     </row>
     <row r="270" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>528</v>
+        <v>557</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>1</v>
@@ -4568,15 +4580,15 @@
     </row>
     <row r="271" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>529</v>
+        <v>558</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>644</v>
+        <v>478</v>
       </c>
     </row>
     <row r="272" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>530</v>
+        <v>559</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>1</v>
@@ -4584,7 +4596,7 @@
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>531</v>
+        <v>560</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>10</v>
@@ -4592,7 +4604,7 @@
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>532</v>
+        <v>561</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>1</v>
@@ -4600,7 +4612,7 @@
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>533</v>
+        <v>562</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>113</v>
@@ -4696,7 +4708,7 @@
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B287" t="s">
-        <v>534</v>
+        <v>563</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>1</v>
@@ -4704,7 +4716,7 @@
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B288" t="s">
-        <v>535</v>
+        <v>564</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>234</v>
@@ -4712,7 +4724,7 @@
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B289" t="s">
-        <v>536</v>
+        <v>565</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>1</v>
@@ -4720,7 +4732,7 @@
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B290" t="s">
-        <v>537</v>
+        <v>566</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>237</v>
@@ -4728,7 +4740,7 @@
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B291" t="s">
-        <v>538</v>
+        <v>567</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>1</v>
@@ -4736,7 +4748,7 @@
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B292" t="s">
-        <v>539</v>
+        <v>568</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>240</v>
@@ -4779,7 +4791,7 @@
         <v>248</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>651</v>
+        <v>485</v>
       </c>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.2">
@@ -4811,7 +4823,7 @@
         <v>252</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>648</v>
+        <v>482</v>
       </c>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.2">
@@ -4827,12 +4839,12 @@
         <v>254</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>652</v>
+        <v>486</v>
       </c>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B304" t="s">
-        <v>540</v>
+        <v>569</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>1</v>
@@ -4840,7 +4852,7 @@
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B305" t="s">
-        <v>541</v>
+        <v>570</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>255</v>
@@ -4848,7 +4860,7 @@
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B306" t="s">
-        <v>542</v>
+        <v>571</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>1</v>
@@ -4856,15 +4868,15 @@
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B307" t="s">
-        <v>543</v>
+        <v>572</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>652</v>
+        <v>486</v>
       </c>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B308" t="s">
-        <v>544</v>
+        <v>573</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>1</v>
@@ -4872,7 +4884,7 @@
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B309" t="s">
-        <v>545</v>
+        <v>574</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>246</v>
@@ -4915,7 +4927,7 @@
         <v>261</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>635</v>
+        <v>469</v>
       </c>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.2">
@@ -4968,7 +4980,7 @@
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B321" t="s">
-        <v>546</v>
+        <v>575</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>1</v>
@@ -4976,7 +4988,7 @@
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B322" t="s">
-        <v>547</v>
+        <v>576</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>27</v>
@@ -4984,7 +4996,7 @@
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B323" t="s">
-        <v>548</v>
+        <v>577</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>1</v>
@@ -4992,7 +5004,7 @@
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B324" t="s">
-        <v>549</v>
+        <v>578</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>15</v>
@@ -5000,7 +5012,7 @@
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B325" t="s">
-        <v>550</v>
+        <v>579</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>1</v>
@@ -5008,7 +5020,7 @@
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B326" t="s">
-        <v>551</v>
+        <v>580</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>1</v>
@@ -5075,7 +5087,7 @@
         <v>276</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>635</v>
+        <v>469</v>
       </c>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.2">
@@ -5128,7 +5140,7 @@
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B341" t="s">
-        <v>552</v>
+        <v>581</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>1</v>
@@ -5136,7 +5148,7 @@
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B342" t="s">
-        <v>553</v>
+        <v>582</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>27</v>
@@ -5144,7 +5156,7 @@
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B343" t="s">
-        <v>554</v>
+        <v>583</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>1</v>
@@ -5152,7 +5164,7 @@
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B344" t="s">
-        <v>555</v>
+        <v>584</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>15</v>
@@ -5160,7 +5172,7 @@
     </row>
     <row r="345" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B345" t="s">
-        <v>556</v>
+        <v>585</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>1</v>
@@ -5168,7 +5180,7 @@
     </row>
     <row r="346" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B346" t="s">
-        <v>557</v>
+        <v>586</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>1</v>
@@ -5288,7 +5300,7 @@
     </row>
     <row r="361" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B361" t="s">
-        <v>558</v>
+        <v>587</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>1</v>
@@ -5296,7 +5308,7 @@
     </row>
     <row r="362" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B362" t="s">
-        <v>559</v>
+        <v>588</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>27</v>
@@ -5304,7 +5316,7 @@
     </row>
     <row r="363" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B363" t="s">
-        <v>560</v>
+        <v>589</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>1</v>
@@ -5312,7 +5324,7 @@
     </row>
     <row r="364" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B364" t="s">
-        <v>561</v>
+        <v>590</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>15</v>
@@ -5320,7 +5332,7 @@
     </row>
     <row r="365" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B365" t="s">
-        <v>562</v>
+        <v>591</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>1</v>
@@ -5328,7 +5340,7 @@
     </row>
     <row r="366" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B366" t="s">
-        <v>563</v>
+        <v>592</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>1</v>
@@ -5448,7 +5460,7 @@
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B381" t="s">
-        <v>564</v>
+        <v>593</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>1</v>
@@ -5456,7 +5468,7 @@
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B382" t="s">
-        <v>565</v>
+        <v>594</v>
       </c>
       <c r="C382" s="1" t="s">
         <v>27</v>
@@ -5464,7 +5476,7 @@
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B383" t="s">
-        <v>566</v>
+        <v>595</v>
       </c>
       <c r="C383" s="1" t="s">
         <v>1</v>
@@ -5472,7 +5484,7 @@
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B384" t="s">
-        <v>567</v>
+        <v>596</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>15</v>
@@ -5480,7 +5492,7 @@
     </row>
     <row r="385" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B385" t="s">
-        <v>568</v>
+        <v>597</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>1</v>
@@ -5488,7 +5500,7 @@
     </row>
     <row r="386" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B386" t="s">
-        <v>569</v>
+        <v>598</v>
       </c>
       <c r="C386" s="1" t="s">
         <v>1</v>
@@ -5555,7 +5567,7 @@
         <v>318</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>653</v>
+        <v>487</v>
       </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.2">
@@ -5608,7 +5620,7 @@
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B401" t="s">
-        <v>570</v>
+        <v>599</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>1</v>
@@ -5616,7 +5628,7 @@
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B402" t="s">
-        <v>571</v>
+        <v>600</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>325</v>
@@ -5624,7 +5636,7 @@
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B403" t="s">
-        <v>572</v>
+        <v>601</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>1</v>
@@ -5632,7 +5644,7 @@
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B404" t="s">
-        <v>573</v>
+        <v>602</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>15</v>
@@ -5640,7 +5652,7 @@
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B405" t="s">
-        <v>574</v>
+        <v>603</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>1</v>
@@ -5648,7 +5660,7 @@
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B406" t="s">
-        <v>575</v>
+        <v>604</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>1</v>
@@ -5768,7 +5780,7 @@
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B421" t="s">
-        <v>576</v>
+        <v>605</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>1</v>
@@ -5776,7 +5788,7 @@
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B422" t="s">
-        <v>577</v>
+        <v>606</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>325</v>
@@ -5784,7 +5796,7 @@
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B423" t="s">
-        <v>578</v>
+        <v>607</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>1</v>
@@ -5792,7 +5804,7 @@
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B424" t="s">
-        <v>579</v>
+        <v>608</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>342</v>
@@ -5800,7 +5812,7 @@
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B425" t="s">
-        <v>580</v>
+        <v>609</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>1</v>
@@ -5808,7 +5820,7 @@
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B426" t="s">
-        <v>581</v>
+        <v>610</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>1</v>
@@ -5928,7 +5940,7 @@
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B441" t="s">
-        <v>582</v>
+        <v>611</v>
       </c>
       <c r="C441" s="1" t="s">
         <v>1</v>
@@ -5936,7 +5948,7 @@
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B442" t="s">
-        <v>583</v>
+        <v>612</v>
       </c>
       <c r="C442" s="1" t="s">
         <v>325</v>
@@ -5944,7 +5956,7 @@
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B443" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>1</v>
@@ -5952,7 +5964,7 @@
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B444" t="s">
-        <v>585</v>
+        <v>614</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>15</v>
@@ -5960,7 +5972,7 @@
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B445" t="s">
-        <v>586</v>
+        <v>615</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>1</v>
@@ -5968,10 +5980,10 @@
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B446" t="s">
-        <v>587</v>
+        <v>616</v>
       </c>
       <c r="C446" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.2">
@@ -6088,7 +6100,7 @@
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B461" t="s">
-        <v>588</v>
+        <v>617</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>1</v>
@@ -6096,7 +6108,7 @@
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B462" t="s">
-        <v>589</v>
+        <v>618</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>374</v>
@@ -6104,7 +6116,7 @@
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B463" t="s">
-        <v>590</v>
+        <v>619</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>1</v>
@@ -6112,7 +6124,7 @@
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B464" t="s">
-        <v>591</v>
+        <v>620</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>15</v>
@@ -6120,7 +6132,7 @@
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B465" t="s">
-        <v>592</v>
+        <v>621</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>1</v>
@@ -6128,10 +6140,10 @@
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B466" t="s">
-        <v>593</v>
+        <v>622</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.2">
@@ -6147,7 +6159,7 @@
         <v>376</v>
       </c>
       <c r="C468" s="1" t="s">
-        <v>654</v>
+        <v>488</v>
       </c>
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.2">
@@ -6195,7 +6207,7 @@
         <v>382</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>654</v>
+        <v>488</v>
       </c>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.2">
@@ -6227,7 +6239,7 @@
         <v>386</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>654</v>
+        <v>488</v>
       </c>
     </row>
     <row r="479" spans="2:3" x14ac:dyDescent="0.2">
@@ -6248,7 +6260,7 @@
     </row>
     <row r="481" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B481" t="s">
-        <v>594</v>
+        <v>623</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>15</v>
@@ -6256,7 +6268,7 @@
     </row>
     <row r="482" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B482" t="s">
-        <v>595</v>
+        <v>624</v>
       </c>
       <c r="C482" s="1" t="s">
         <v>1</v>
@@ -6264,7 +6276,7 @@
     </row>
     <row r="483" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B483" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="C483" s="1" t="s">
         <v>1</v>
@@ -6272,15 +6284,15 @@
     </row>
     <row r="484" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B484" t="s">
-        <v>597</v>
+        <v>626</v>
       </c>
       <c r="C484" s="1" t="s">
-        <v>655</v>
+        <v>489</v>
       </c>
     </row>
     <row r="485" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B485" t="s">
-        <v>598</v>
+        <v>627</v>
       </c>
       <c r="C485" s="1" t="s">
         <v>15</v>
@@ -6288,7 +6300,7 @@
     </row>
     <row r="486" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B486" t="s">
-        <v>599</v>
+        <v>628</v>
       </c>
       <c r="C486" s="1" t="s">
         <v>1</v>
@@ -6376,7 +6388,7 @@
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B497" t="s">
-        <v>600</v>
+        <v>629</v>
       </c>
       <c r="C497" s="1" t="s">
         <v>1</v>
@@ -6384,7 +6396,7 @@
     </row>
     <row r="498" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B498" t="s">
-        <v>601</v>
+        <v>630</v>
       </c>
       <c r="C498" s="1" t="s">
         <v>1</v>
@@ -6392,7 +6404,7 @@
     </row>
     <row r="499" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B499" t="s">
-        <v>602</v>
+        <v>631</v>
       </c>
       <c r="C499" s="1" t="s">
         <v>1</v>
@@ -6400,7 +6412,7 @@
     </row>
     <row r="500" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B500" t="s">
-        <v>603</v>
+        <v>632</v>
       </c>
       <c r="C500" s="1" t="s">
         <v>1</v>
@@ -6408,7 +6420,7 @@
     </row>
     <row r="501" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B501" t="s">
-        <v>604</v>
+        <v>633</v>
       </c>
       <c r="C501" s="1" t="s">
         <v>1</v>
@@ -6416,7 +6428,7 @@
     </row>
     <row r="502" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B502" t="s">
-        <v>605</v>
+        <v>634</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>1</v>
@@ -6475,7 +6487,7 @@
         <v>406</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>655</v>
+        <v>489</v>
       </c>
     </row>
     <row r="510" spans="2:3" x14ac:dyDescent="0.2">
@@ -6504,7 +6516,7 @@
     </row>
     <row r="513" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B513" t="s">
-        <v>606</v>
+        <v>635</v>
       </c>
       <c r="C513" s="1" t="s">
         <v>1</v>
@@ -6512,7 +6524,7 @@
     </row>
     <row r="514" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B514" t="s">
-        <v>607</v>
+        <v>636</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>325</v>
@@ -6520,7 +6532,7 @@
     </row>
     <row r="515" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B515" t="s">
-        <v>608</v>
+        <v>637</v>
       </c>
       <c r="C515" s="1" t="s">
         <v>1</v>
@@ -6528,7 +6540,7 @@
     </row>
     <row r="516" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B516" t="s">
-        <v>609</v>
+        <v>638</v>
       </c>
       <c r="C516" s="1" t="s">
         <v>1</v>
@@ -6536,7 +6548,7 @@
     </row>
     <row r="517" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B517" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
       <c r="C517" s="1" t="s">
         <v>1</v>
@@ -6544,7 +6556,7 @@
     </row>
     <row r="518" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B518" t="s">
-        <v>611</v>
+        <v>640</v>
       </c>
       <c r="C518" s="1" t="s">
         <v>1</v>
@@ -6647,19 +6659,43 @@
       </c>
     </row>
     <row r="531" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>462</v>
+      </c>
       <c r="B531" t="s">
         <v>423</v>
       </c>
       <c r="C531" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D531" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E531" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F531" s="1" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="532" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>461</v>
+      </c>
       <c r="B532" t="s">
         <v>424</v>
       </c>
       <c r="C532" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E532" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F532" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="533" spans="1:6" x14ac:dyDescent="0.2">
@@ -6696,10 +6732,10 @@
         <v>427</v>
       </c>
       <c r="E534" s="1" t="s">
-        <v>642</v>
+        <v>476</v>
       </c>
       <c r="F534" s="1" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.2">
@@ -6720,7 +6756,7 @@
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B537" t="s">
-        <v>612</v>
+        <v>641</v>
       </c>
       <c r="C537" s="1" t="s">
         <v>15</v>
@@ -6728,7 +6764,7 @@
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B538" t="s">
-        <v>613</v>
+        <v>642</v>
       </c>
       <c r="C538" s="1" t="s">
         <v>1</v>
@@ -6736,7 +6772,7 @@
     </row>
     <row r="539" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B539" t="s">
-        <v>614</v>
+        <v>643</v>
       </c>
       <c r="C539" s="1" t="s">
         <v>1</v>
@@ -6744,7 +6780,7 @@
     </row>
     <row r="540" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B540" t="s">
-        <v>615</v>
+        <v>644</v>
       </c>
       <c r="C540" s="1" t="s">
         <v>427</v>
@@ -6752,7 +6788,7 @@
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B541" t="s">
-        <v>616</v>
+        <v>645</v>
       </c>
       <c r="C541" s="1" t="s">
         <v>15</v>
@@ -6760,10 +6796,10 @@
     </row>
     <row r="542" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B542" t="s">
-        <v>617</v>
+        <v>646</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>655</v>
+        <v>489</v>
       </c>
     </row>
     <row r="543" spans="1:6" x14ac:dyDescent="0.2">
@@ -6848,7 +6884,7 @@
     </row>
     <row r="553" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B553" t="s">
-        <v>618</v>
+        <v>647</v>
       </c>
       <c r="C553" s="1" t="s">
         <v>1</v>
@@ -6856,15 +6892,15 @@
     </row>
     <row r="554" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B554" t="s">
-        <v>619</v>
+        <v>648</v>
       </c>
       <c r="C554" s="1" t="s">
-        <v>655</v>
+        <v>489</v>
       </c>
     </row>
     <row r="555" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B555" t="s">
-        <v>620</v>
+        <v>649</v>
       </c>
       <c r="C555" s="1" t="s">
         <v>15</v>
@@ -6872,7 +6908,7 @@
     </row>
     <row r="556" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B556" t="s">
-        <v>621</v>
+        <v>650</v>
       </c>
       <c r="C556" s="1" t="s">
         <v>440</v>
@@ -6880,7 +6916,7 @@
     </row>
     <row r="557" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B557" t="s">
-        <v>622</v>
+        <v>651</v>
       </c>
       <c r="C557" s="1" t="s">
         <v>1</v>
@@ -6888,7 +6924,7 @@
     </row>
     <row r="558" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B558" t="s">
-        <v>623</v>
+        <v>652</v>
       </c>
       <c r="C558" s="1" t="s">
         <v>1</v>
@@ -6976,7 +7012,7 @@
     </row>
     <row r="569" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B569" t="s">
-        <v>624</v>
+        <v>653</v>
       </c>
       <c r="C569" s="1" t="s">
         <v>1</v>
@@ -6984,7 +7020,7 @@
     </row>
     <row r="570" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B570" t="s">
-        <v>625</v>
+        <v>654</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>1</v>
@@ -6992,7 +7028,7 @@
     </row>
     <row r="571" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B571" t="s">
-        <v>626</v>
+        <v>655</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>15</v>
@@ -7000,7 +7036,7 @@
     </row>
     <row r="572" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B572" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>1</v>
@@ -7008,7 +7044,7 @@
     </row>
     <row r="573" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B573" t="s">
-        <v>628</v>
+        <v>657</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>15</v>
@@ -7016,7 +7052,7 @@
     </row>
     <row r="574" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B574" t="s">
-        <v>629</v>
+        <v>658</v>
       </c>
       <c r="C574" s="1" t="s">
         <v>1</v>
@@ -7040,7 +7076,7 @@
     </row>
     <row r="577" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B577" t="s">
-        <v>630</v>
+        <v>659</v>
       </c>
       <c r="C577" s="1" t="s">
         <v>1</v>

</xml_diff>